<commit_message>
fixed motor sync in measurements tab
</commit_message>
<xml_diff>
--- a/tst.xlsx
+++ b/tst.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,10 +483,10 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>46011.97013636221</v>
+        <v>46012.00663381386</v>
       </c>
       <c r="B2" t="n">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -497,10 +497,10 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>104.746025176778</v>
+        <v>102.7864362949354</v>
       </c>
       <c r="F2" t="n">
-        <v>100.2914098052421</v>
+        <v>103.6176719758972</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -508,6 +508,636 @@
         </is>
       </c>
       <c r="H2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>46012.00663600706</v>
+      </c>
+      <c r="B3" t="n">
+        <v>378</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E3" t="n">
+        <v>102.2417100825305</v>
+      </c>
+      <c r="F3" t="n">
+        <v>103.5172487110082</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>neg_from_zero</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>46012.00663817136</v>
+      </c>
+      <c r="B4" t="n">
+        <v>565</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>-2</v>
+      </c>
+      <c r="E4" t="n">
+        <v>102.5133369128759</v>
+      </c>
+      <c r="F4" t="n">
+        <v>103.6627063416886</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>neg_from_zero</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
+        <v>46012.00664034129</v>
+      </c>
+      <c r="B5" t="n">
+        <v>753</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>-3</v>
+      </c>
+      <c r="E5" t="n">
+        <v>102.4680167000933</v>
+      </c>
+      <c r="F5" t="n">
+        <v>102.7521702381491</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>neg_from_zero</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>46012.00664250603</v>
+      </c>
+      <c r="B6" t="n">
+        <v>940</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>-4</v>
+      </c>
+      <c r="E6" t="n">
+        <v>101.787619615254</v>
+      </c>
+      <c r="F6" t="n">
+        <v>102.3644131340291</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>neg_from_zero</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>46012.00664485617</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1143</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>-5</v>
+      </c>
+      <c r="E7" t="n">
+        <v>101.3463428410157</v>
+      </c>
+      <c r="F7" t="n">
+        <v>102.4700755743888</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>neg_from_zero</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
+        <v>46012.00664701962</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1330</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>-6</v>
+      </c>
+      <c r="E8" t="n">
+        <v>100.927456385969</v>
+      </c>
+      <c r="F8" t="n">
+        <v>101.8146031367819</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>neg_from_zero</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
+        <v>46012.00664915697</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1515</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>-7</v>
+      </c>
+      <c r="E9" t="n">
+        <v>101.3201510496824</v>
+      </c>
+      <c r="F9" t="n">
+        <v>101.808546349741</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>neg_from_zero</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>46012.00665132901</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1702</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>-8</v>
+      </c>
+      <c r="E10" t="n">
+        <v>100.6510293254725</v>
+      </c>
+      <c r="F10" t="n">
+        <v>101.4892014435307</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>neg_from_zero</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
+        <v>46012.00665367036</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1905</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>-9</v>
+      </c>
+      <c r="E11" t="n">
+        <v>100.9768495825334</v>
+      </c>
+      <c r="F11" t="n">
+        <v>100.5091010188796</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>neg_from_zero</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n">
+        <v>46012.0066558497</v>
+      </c>
+      <c r="B12" t="n">
+        <v>2093</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>-10</v>
+      </c>
+      <c r="E12" t="n">
+        <v>100.7251152063457</v>
+      </c>
+      <c r="F12" t="n">
+        <v>100.8274453861191</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>neg_from_zero</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="n">
+        <v>46012.00665798802</v>
+      </c>
+      <c r="B13" t="n">
+        <v>2278</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>-11</v>
+      </c>
+      <c r="E13" t="n">
+        <v>100.0138012012044</v>
+      </c>
+      <c r="F13" t="n">
+        <v>99.91583107641959</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>neg_from_zero</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="n">
+        <v>46012.00666017957</v>
+      </c>
+      <c r="B14" t="n">
+        <v>2467</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>-12</v>
+      </c>
+      <c r="E14" t="n">
+        <v>100.378633553606</v>
+      </c>
+      <c r="F14" t="n">
+        <v>99.71872289754515</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>neg_from_zero</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="n">
+        <v>46012.00666216741</v>
+      </c>
+      <c r="B15" t="n">
+        <v>2639</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>-13</v>
+      </c>
+      <c r="E15" t="n">
+        <v>99.28545945632472</v>
+      </c>
+      <c r="F15" t="n">
+        <v>99.13564467296975</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>neg_from_zero</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="n">
+        <v>46012.00666434348</v>
+      </c>
+      <c r="B16" t="n">
+        <v>2827</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>-14</v>
+      </c>
+      <c r="E16" t="n">
+        <v>99.79118000140878</v>
+      </c>
+      <c r="F16" t="n">
+        <v>99.26840504381893</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>neg_from_zero</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="n">
+        <v>46012.00666650035</v>
+      </c>
+      <c r="B17" t="n">
+        <v>3013</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>-15</v>
+      </c>
+      <c r="E17" t="n">
+        <v>99.50682228806215</v>
+      </c>
+      <c r="F17" t="n">
+        <v>99.02671514116204</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>neg_from_zero</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="n">
+        <v>46012.00666866509</v>
+      </c>
+      <c r="B18" t="n">
+        <v>3200</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>-16</v>
+      </c>
+      <c r="E18" t="n">
+        <v>98.99461218779736</v>
+      </c>
+      <c r="F18" t="n">
+        <v>98.90496479787578</v>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>neg_from_zero</t>
+        </is>
+      </c>
+      <c r="H18" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="n">
+        <v>46012.00667082192</v>
+      </c>
+      <c r="B19" t="n">
+        <v>3386</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>-17</v>
+      </c>
+      <c r="E19" t="n">
+        <v>98.6011456908239</v>
+      </c>
+      <c r="F19" t="n">
+        <v>98.12518495745687</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>neg_from_zero</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="n">
+        <v>46012.00667297755</v>
+      </c>
+      <c r="B20" t="n">
+        <v>3573</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>-18</v>
+      </c>
+      <c r="E20" t="n">
+        <v>98.82210925962336</v>
+      </c>
+      <c r="F20" t="n">
+        <v>97.83944941013125</v>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>neg_from_zero</t>
+        </is>
+      </c>
+      <c r="H20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="n">
+        <v>46012.0066751592</v>
+      </c>
+      <c r="B21" t="n">
+        <v>3761</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>-19</v>
+      </c>
+      <c r="E21" t="n">
+        <v>98.62932765572002</v>
+      </c>
+      <c r="F21" t="n">
+        <v>97.4504664320563</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>neg_from_zero</t>
+        </is>
+      </c>
+      <c r="H21" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="n">
+        <v>46012.00667748795</v>
+      </c>
+      <c r="B22" t="n">
+        <v>3962</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>-20</v>
+      </c>
+      <c r="E22" t="n">
+        <v>98.24053960292007</v>
+      </c>
+      <c r="F22" t="n">
+        <v>96.55702531265624</v>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>neg_from_zero</t>
+        </is>
+      </c>
+      <c r="H22" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="n">
+        <v>46012.00668196869</v>
+      </c>
+      <c r="B23" t="n">
+        <v>4350</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>-21</v>
+      </c>
+      <c r="E23" t="n">
+        <v>97.3490239078785</v>
+      </c>
+      <c r="F23" t="n">
+        <v>96.13854733236398</v>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>neg_from_zero</t>
+        </is>
+      </c>
+      <c r="H23" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>